<commit_message>
Updated code on timestamp:   16-01-2022 - 13:48:44.34
</commit_message>
<xml_diff>
--- a/Level2.xlsx
+++ b/Level2.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C370D2DD-3D1B-480F-BB67-33EB018971FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7DF9A19-0173-46FC-9E90-B4313CA6EA77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="recursion-and-backtracking" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="399">
   <si>
     <t> Abbreviation Using Backtracking Medium</t>
   </si>
@@ -1214,13 +1214,25 @@
   </si>
   <si>
     <t> Maximum Number Of 1's Row</t>
+  </si>
+  <si>
+    <t> Is A Power Of 4 Easy</t>
+  </si>
+  <si>
+    <t> Xor Queries Of A Subarray Medium</t>
+  </si>
+  <si>
+    <t> Minimum Flips To Make A Or B Equal To C Easy</t>
+  </si>
+  <si>
+    <t> Find Longest Awesome Substring Medium</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1236,16 +1248,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1253,15 +1279,70 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1989,7 +2070,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A2:B37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
@@ -2326,18 +2407,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:B32"/>
+  <dimension ref="A2:E37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="46" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -2345,280 +2428,352 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="5" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="6" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="6" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="6" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="6" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="6" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="6" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="6" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="7" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" s="2"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" s="2"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" s="2"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" s="2"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" s="2"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" s="2"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" s="2"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="C26" s="2"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" s="2"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B30" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B31" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>77</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>398</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/basics-of-bit-official/ojquestion" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="B4" r:id="rId2" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/print-value-of-rsb-mask-official/ojquestion" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="B5" r:id="rId3" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/kernighans-algo-official/ojquestion" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="B6" r:id="rId4" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/josephus-special-official/ojquestion" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="B7" r:id="rId5" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/gray-code/ojquestion" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="B8" r:id="rId6" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/minimum-number-of-software-developers-official/ojquestion" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
-    <hyperlink ref="B9" r:id="rId7" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/number-of-valid-words-official/ojquestion" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
-    <hyperlink ref="B10" r:id="rId8" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/all-repeating-except-one-official/ojquestion" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
-    <hyperlink ref="B11" r:id="rId9" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/all-repeating-except-two-official/ojquestion" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
-    <hyperlink ref="B12" r:id="rId10" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/one-repeating-and-one-missing-official/ojquestion" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
-    <hyperlink ref="B13" r:id="rId11" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/all-repeating-three-times-except-one-official/ojquestion" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
-    <hyperlink ref="B14" r:id="rId12" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/triplets-1-official/ojquestion" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
-    <hyperlink ref="B15" r:id="rId13" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/reduce-n-to-1-official/ojquestion" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
-    <hyperlink ref="B16" r:id="rId14" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/pepcoder-and-bits-official/ojquestion" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
-    <hyperlink ref="B17" r:id="rId15" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/xor-sum-pair-official/ojquestion" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
-    <hyperlink ref="B18" r:id="rId16" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/abrreviation1-using-bits-official/ojquestion" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
-    <hyperlink ref="B19" r:id="rId17" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/utf-8-encoding-official/ojquestion" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
-    <hyperlink ref="B20" r:id="rId18" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/sudoku-using-bit-manipulation-official/ojquestion" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
-    <hyperlink ref="B21" r:id="rId19" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/nqueens-using-bits-official/ojquestion" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
-    <hyperlink ref="B22" r:id="rId20" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/flip-bits-to-convert-a-to-b-official/ojquestion" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
-    <hyperlink ref="B23" r:id="rId21" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/copy-set-bits-in-a-range-official/ojquestion" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
-    <hyperlink ref="B24" r:id="rId22" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/is-a-power-of-2-official/ojquestion" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
-    <hyperlink ref="B25" r:id="rId23" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/solve-7nby8-official/ojquestion" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
-    <hyperlink ref="B26" r:id="rId24" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/swap-all-odd-and-even-bits-official/ojquestion" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
-    <hyperlink ref="B27" r:id="rId25" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/sum-of-bit-differences-of-all-pairs-official/ojquestion" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
-    <hyperlink ref="B28" r:id="rId26" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/check-divisibility-by-3-official/ojquestion" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
-    <hyperlink ref="B29" r:id="rId27" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/count-setbits-in-first-n-natural-numbers-official/ojquestion" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
-    <hyperlink ref="B30" r:id="rId28" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/print-binary-and-reverse-bits-official/ojquestion" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
-    <hyperlink ref="B31" r:id="rId29" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/min-xor-pairs-official/ojquestion" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
-    <hyperlink ref="B32" r:id="rId30" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/nth-palindromic-binary-official/ojquestion" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
+    <hyperlink ref="B3" r:id="rId1" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/basics-of-bit-official/ojquestion" xr:uid="{855BA9E0-FACA-4306-8A78-672F5D625323}"/>
+    <hyperlink ref="B4" r:id="rId2" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/print-value-of-rsb-mask-official/ojquestion" xr:uid="{1C9E0F74-BC32-4FFE-9F88-4237402E2B5C}"/>
+    <hyperlink ref="B5" r:id="rId3" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/kernighans-algo-official/ojquestion" xr:uid="{DBF8203D-F78D-4BC6-A1F9-809423A15DC7}"/>
+    <hyperlink ref="B6" r:id="rId4" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/josephus-special-official/ojquestion" xr:uid="{42503A9E-DD31-4907-A9A9-3B6F50BDF6E0}"/>
+    <hyperlink ref="B7" r:id="rId5" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/gray-code/ojquestion" xr:uid="{C8258836-C1B6-4B0D-9D21-E6DFC1F524F3}"/>
+    <hyperlink ref="B8" r:id="rId6" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/minimum-number-of-software-developers-official/ojquestion" xr:uid="{6AD4CBC5-D4D6-4F6B-BE63-99BB72FDAC43}"/>
+    <hyperlink ref="B9" r:id="rId7" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/number-of-valid-words-official/ojquestion" xr:uid="{D0AD348B-906A-4995-AB72-313196A5E580}"/>
+    <hyperlink ref="B10" r:id="rId8" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/all-repeating-except-one-official/ojquestion" xr:uid="{F43086ED-8748-4BFA-B1EA-917B42B56F0C}"/>
+    <hyperlink ref="B11" r:id="rId9" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/all-repeating-except-two-official/ojquestion" xr:uid="{E396097F-0915-46FB-9C01-983D188697B2}"/>
+    <hyperlink ref="B12" r:id="rId10" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/one-repeating-and-one-missing-official/ojquestion" xr:uid="{0357CAAF-2635-4039-878F-98B75EBC2FFA}"/>
+    <hyperlink ref="B13" r:id="rId11" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/all-repeating-three-times-except-one-official/ojquestion" xr:uid="{E6717FCA-65B0-4402-AF64-90030D33CD24}"/>
+    <hyperlink ref="B14" r:id="rId12" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/triplets-1-official/ojquestion" xr:uid="{35997945-A200-401A-B23B-991CFA6A6FF0}"/>
+    <hyperlink ref="B15" r:id="rId13" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/reduce-n-to-1-official/ojquestion" xr:uid="{87C9CDA8-BD0B-473E-A27D-58F795067608}"/>
+    <hyperlink ref="B16" r:id="rId14" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/pepcoder-and-bits-official/ojquestion" xr:uid="{FDBB304B-B31E-446C-884E-DA4B001A7F70}"/>
+    <hyperlink ref="B17" r:id="rId15" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/xor-sum-pair-official/ojquestion" xr:uid="{97F574AD-1AB9-498E-9267-A533EFE0F368}"/>
+    <hyperlink ref="B18" r:id="rId16" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/abrreviation1-using-bits-official/ojquestion" xr:uid="{C9575ABC-03A1-4AC9-A133-D48116FE2821}"/>
+    <hyperlink ref="B19" r:id="rId17" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/utf-8-encoding-official/ojquestion" xr:uid="{9D4D0B06-8A63-476D-9B76-DF8387601064}"/>
+    <hyperlink ref="B20" r:id="rId18" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/sudoku-using-bit-manipulation-official/ojquestion" xr:uid="{0C56D1A5-F8E5-4B93-9A61-3849773AA1E6}"/>
+    <hyperlink ref="B21" r:id="rId19" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/nqueens-using-bits-official/ojquestion" xr:uid="{A07BAA3C-3F0C-4D59-9375-9B65FB95EB5F}"/>
+    <hyperlink ref="B22" r:id="rId20" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/flip-bits-to-convert-a-to-b-official/ojquestion" xr:uid="{C610C2D1-5747-477E-851B-1646DB17E635}"/>
+    <hyperlink ref="B23" r:id="rId21" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/flip-bits-to-convert-a-to-b-official/ojquestion" xr:uid="{66572DE4-E2B8-4E55-B5CA-B27251A92629}"/>
+    <hyperlink ref="B24" r:id="rId22" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/copy-set-bits-in-a-range-official/ojquestion" xr:uid="{02A01CAC-7892-4B94-B3DE-41FB2E26C200}"/>
+    <hyperlink ref="B25" r:id="rId23" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/is-a-power-of-2-official/ojquestion" xr:uid="{E8A38ED6-F94A-47FB-9B5D-22C15E5D9139}"/>
+    <hyperlink ref="B26" r:id="rId24" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/is-a-power-of-4/ojquestion" xr:uid="{2015037F-138C-4368-8206-EFB0A7CFA461}"/>
+    <hyperlink ref="B27" r:id="rId25" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/solve-7nby8-official/ojquestion" xr:uid="{AF96BE46-2135-4D92-996D-73F6AC2657C8}"/>
+    <hyperlink ref="B28" r:id="rId26" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/swap-all-odd-and-even-bits-official/ojquestion" xr:uid="{23AEE5F4-05B4-4D8E-9C4A-7C2D601273D5}"/>
+    <hyperlink ref="B29" r:id="rId27" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/sum-of-bit-differences-of-all-pairs-official/ojquestion" xr:uid="{E8F55F46-55C3-4680-AFEA-DEC53D747D36}"/>
+    <hyperlink ref="B30" r:id="rId28" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/check-divisibility-by-3-official/ojquestion" xr:uid="{20B77BFD-C372-42B3-89D4-0BAF1BB2A298}"/>
+    <hyperlink ref="B31" r:id="rId29" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/count-setbits-in-first-n-natural-numbers-official/ojquestion" xr:uid="{84A4BD7D-0C5E-4FBE-90DA-0692B543096D}"/>
+    <hyperlink ref="B32" r:id="rId30" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/print-binary-and-reverse-bits-official/ojquestion" xr:uid="{8F87BCAB-375D-4180-ACB6-38AAE99CF2AC}"/>
+    <hyperlink ref="B33" r:id="rId31" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/min-xor-pairs-official/ojquestion" xr:uid="{4C3B1C78-1666-48A3-84F0-16BF1E6F44B6}"/>
+    <hyperlink ref="B34" r:id="rId32" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/nth-palindromic-binary-official/ojquestion" xr:uid="{F451D6AC-8742-45FE-B3B6-23C12EB1D9FF}"/>
+    <hyperlink ref="B35" r:id="rId33" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/bit-manipulation-xor-qs/ojquestion" xr:uid="{5097BD36-57F7-4B97-85F1-17F17067B2D0}"/>
+    <hyperlink ref="B36" r:id="rId34" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/minimum-flips-abc/ojquestion" xr:uid="{C231DE90-6011-446F-8C90-5DCE3DCF9C54}"/>
+    <hyperlink ref="B37" r:id="rId35" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/find-longest-awesome-substring/ojquestion" xr:uid="{24D7352B-246C-494A-B01F-B134E6A4D40D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId36"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated code on timestamp:   15-06-2022 - 22:30:36.90
</commit_message>
<xml_diff>
--- a/Level2.xlsx
+++ b/Level2.xlsx
@@ -3,25 +3,26 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59B08D8-67A2-4883-839E-1C14A98E9033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BD1B8EC-ED2A-4EA7-9FE7-EF0BBDE592C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="recursion-and-backtracking" sheetId="1" r:id="rId1"/>
     <sheet name="bit-manipulation" sheetId="2" r:id="rId2"/>
     <sheet name="dynamic-programming" sheetId="3" r:id="rId3"/>
-    <sheet name="Trees" sheetId="4" r:id="rId4"/>
+    <sheet name="graph" sheetId="6" r:id="rId4"/>
     <sheet name="Hashmap &amp; heap" sheetId="5" r:id="rId5"/>
-    <sheet name="graph" sheetId="6" r:id="rId6"/>
-    <sheet name="Stack" sheetId="7" r:id="rId7"/>
-    <sheet name="Trie" sheetId="11" r:id="rId8"/>
-    <sheet name="LL" sheetId="8" r:id="rId9"/>
+    <sheet name="Trees" sheetId="4" r:id="rId6"/>
+    <sheet name="LL" sheetId="8" r:id="rId7"/>
+    <sheet name="Stack" sheetId="7" r:id="rId8"/>
+    <sheet name="Trie" sheetId="11" r:id="rId9"/>
     <sheet name="ARRAY" sheetId="9" r:id="rId10"/>
     <sheet name="SearchSort" sheetId="10" r:id="rId11"/>
     <sheet name="Misc" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="541">
   <si>
     <t> Abbreviation Using Backtracking Medium</t>
   </si>
@@ -1651,6 +1652,9 @@
   </si>
   <si>
     <t> Heap - Comparable V/s Comparator</t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
@@ -2443,8 +2447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A2:B79"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B79"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40:A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2781,186 +2785,297 @@
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>41</v>
+      </c>
       <c r="B43" s="2" t="s">
         <v>471</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>42</v>
+      </c>
       <c r="B44" s="2" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>43</v>
+      </c>
       <c r="B45" s="2" t="s">
         <v>472</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>44</v>
+      </c>
       <c r="B46" s="2" t="s">
         <v>473</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>45</v>
+      </c>
       <c r="B47" s="2" t="s">
         <v>474</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>46</v>
+      </c>
       <c r="B48" s="2" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>47</v>
+      </c>
       <c r="B49" s="2" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>48</v>
+      </c>
       <c r="B50" s="2" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>49</v>
+      </c>
       <c r="B51" s="2" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>50</v>
+      </c>
       <c r="B52" s="2" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>51</v>
+      </c>
       <c r="B53" s="2" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>52</v>
+      </c>
       <c r="B54" s="2" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>53</v>
+      </c>
       <c r="B55" s="2" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>54</v>
+      </c>
       <c r="B56" s="2" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>55</v>
+      </c>
       <c r="B57" s="2" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>56</v>
+      </c>
       <c r="B58" s="2" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>57</v>
+      </c>
       <c r="B59" s="2" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>58</v>
+      </c>
       <c r="B60" s="2" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>59</v>
+      </c>
       <c r="B61" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>60</v>
+      </c>
       <c r="B62" s="2" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>61</v>
+      </c>
       <c r="B63" s="2" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>62</v>
+      </c>
       <c r="B64" s="2" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>63</v>
+      </c>
       <c r="B65" s="2" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>64</v>
+      </c>
       <c r="B66" s="2" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>65</v>
+      </c>
       <c r="B67" s="2" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>66</v>
+      </c>
       <c r="B68" s="2" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>67</v>
+      </c>
       <c r="B69" s="2" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>68</v>
+      </c>
       <c r="B70" s="2" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>69</v>
+      </c>
       <c r="B71" s="2" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>70</v>
+      </c>
       <c r="B72" s="2" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>71</v>
+      </c>
       <c r="B73" s="2" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>72</v>
+      </c>
       <c r="B74" s="2" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>73</v>
+      </c>
       <c r="B75" s="2" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>74</v>
+      </c>
       <c r="B76" s="2" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>75</v>
+      </c>
       <c r="B77" s="2" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>76</v>
+      </c>
       <c r="B78" s="2" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>77</v>
+      </c>
       <c r="B79" s="2" t="s">
         <v>495</v>
       </c>
@@ -3053,8 +3168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A2:B47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B47"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36:A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3351,51 +3466,81 @@
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>36</v>
+      </c>
       <c r="B38" s="2" t="s">
         <v>517</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>37</v>
+      </c>
       <c r="B39" s="2" t="s">
         <v>518</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>38</v>
+      </c>
       <c r="B40" s="2" t="s">
         <v>519</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>39</v>
+      </c>
       <c r="B41" s="2" t="s">
         <v>520</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>40</v>
+      </c>
       <c r="B42" s="2" t="s">
         <v>521</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>41</v>
+      </c>
       <c r="B43" s="2" t="s">
         <v>522</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>42</v>
+      </c>
       <c r="B44" s="2" t="s">
         <v>523</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>43</v>
+      </c>
       <c r="B45" s="2" t="s">
         <v>524</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>44</v>
+      </c>
       <c r="B46" s="2" t="s">
         <v>525</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>45</v>
+      </c>
       <c r="B47" s="2" t="s">
         <v>526</v>
       </c>
@@ -3456,7 +3601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09BB8B39-CED0-4239-A937-46214D1FA8AA}">
   <dimension ref="B3:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3:B15"/>
     </sheetView>
   </sheetViews>
@@ -4668,16 +4813,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A2:B59"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A2:B42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B59"/>
+      <selection activeCell="A12" sqref="A12:A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="64.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -4693,7 +4838,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>177</v>
+        <v>361</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -4701,7 +4846,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>178</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -4709,7 +4854,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -4717,7 +4862,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -4725,7 +4870,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>156</v>
+        <v>362</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -4733,7 +4878,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>157</v>
+        <v>363</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -4741,7 +4886,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>158</v>
+        <v>364</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -4749,7 +4894,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>159</v>
+        <v>365</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -4757,15 +4902,15 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>410</v>
+        <v>367</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -4773,7 +4918,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>411</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -4781,7 +4926,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -4789,7 +4934,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>162</v>
+        <v>368</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -4797,7 +4942,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>163</v>
+        <v>369</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -4805,7 +4950,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>164</v>
+        <v>370</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -4813,7 +4958,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>165</v>
+        <v>371</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -4821,7 +4966,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>412</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -4829,7 +4974,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>166</v>
+        <v>144</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -4837,7 +4982,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>167</v>
+        <v>145</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -4845,7 +4990,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>168</v>
+        <v>148</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -4853,7 +4998,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -4861,7 +5006,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>170</v>
+        <v>372</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -4869,15 +5014,15 @@
         <v>23</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>172</v>
+        <v>374</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -4885,7 +5030,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>173</v>
+        <v>375</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -4893,7 +5038,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>174</v>
+        <v>376</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -4901,7 +5046,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>175</v>
+        <v>377</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -4909,7 +5054,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>176</v>
+        <v>378</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -4917,7 +5062,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>179</v>
+        <v>379</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -4925,7 +5070,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>180</v>
+        <v>380</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -4933,7 +5078,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>181</v>
+        <v>381</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -4941,193 +5086,115 @@
         <v>32</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>33</v>
+      </c>
       <c r="B35" s="2" t="s">
-        <v>413</v>
+        <v>383</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>34</v>
+      </c>
       <c r="B36" s="2" t="s">
-        <v>414</v>
+        <v>384</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>35</v>
+      </c>
       <c r="B37" s="2" t="s">
-        <v>415</v>
+        <v>385</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>36</v>
+      </c>
       <c r="B38" s="2" t="s">
-        <v>416</v>
+        <v>386</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>37</v>
+      </c>
       <c r="B39" s="2" t="s">
-        <v>417</v>
+        <v>387</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>38</v>
+      </c>
       <c r="B40" s="2" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>39</v>
+      </c>
       <c r="B41" s="2" t="s">
-        <v>419</v>
+        <v>389</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>40</v>
+      </c>
       <c r="B42" s="2" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B43" s="2" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B44" s="2" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B45" s="2" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B46" s="2" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B47" s="2" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B48" s="2" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B49" s="2" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B50" s="2" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B51" s="2" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B52" s="2" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B53" s="2" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B54" s="2" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B55" s="2" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B56" s="2" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B57" s="2" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B58" s="2" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B59" s="2" t="s">
-        <v>437</v>
+        <v>390</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/in-order-morris-traversal-in-binarytree/ojquestion" xr:uid="{12FE414D-86EC-4703-89B8-46439B34D434}"/>
-    <hyperlink ref="B4" r:id="rId2" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/pre-order-morris-traversal-in-binary-tree/ojquestion" xr:uid="{08B75074-0749-4158-B777-D7C28A447CDD}"/>
-    <hyperlink ref="B5" r:id="rId3" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/cameras-in-binary-tree-official/ojquestion" xr:uid="{766A30BC-D241-4F59-9799-3F802861EFA8}"/>
-    <hyperlink ref="B6" r:id="rId4" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/levelup_house-robber-in-binary-tree/ojquestion" xr:uid="{5006CB72-6882-4AF8-B797-ECC3B3688491}"/>
-    <hyperlink ref="B7" r:id="rId5" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/longest-zigzag-path-in-a-binary-tree/ojquestion" xr:uid="{71FF4B48-68F7-4A31-9152-1A98444F8F1C}"/>
-    <hyperlink ref="B8" r:id="rId6" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/levelup_validate-bst/ojquestion" xr:uid="{2376104C-A4E1-4B92-A733-4EE741230FC5}"/>
-    <hyperlink ref="B9" r:id="rId7" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/recover-bst/ojquestion" xr:uid="{BA60A109-AAF7-4998-BBA5-13BCB53EDC8D}"/>
-    <hyperlink ref="B10" r:id="rId8" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/construct-binarytree-from-preorder-and-inorder-traversal/ojquestion" xr:uid="{36463C2E-5A17-437B-865D-4051FDD5C52E}"/>
-    <hyperlink ref="B11" r:id="rId9" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/construct-binarytree-from-postorder-and-inorder-traversal/ojquestion" xr:uid="{936FAD46-6EB8-4AB6-9CA8-AA7BCE58678D}"/>
-    <hyperlink ref="B12" r:id="rId10" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/construct-binarytree-from-inorder-and-levelorder-traversal/ojquestion" xr:uid="{12969EDF-DA52-4F3B-A353-43B0D8E2AD8C}"/>
-    <hyperlink ref="B13" r:id="rId11" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/construct-binary-tree-from-levelorder-and-inorder-traversal/ojquestion" xr:uid="{AFEF680C-5099-489D-8DE5-D926E37189F5}"/>
-    <hyperlink ref="B14" r:id="rId12" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/construct-bst-from-inorder-traversal/ojquestion" xr:uid="{C7E3583C-89E4-4578-AD50-49378E673B2D}"/>
-    <hyperlink ref="B15" r:id="rId13" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/construct-bst-from-preorder-traversal/ojquestion" xr:uid="{70A85115-3368-4BDB-BEF6-5D7CA73E256A}"/>
-    <hyperlink ref="B16" r:id="rId14" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/construct-bst-from-postorder-traversal/ojquestion" xr:uid="{232E7B35-A67D-4094-AED1-925211E5CE54}"/>
-    <hyperlink ref="B17" r:id="rId15" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/construct-bst-from-levelorder-traversal/ojquestion" xr:uid="{42913B87-06BD-4CC0-98B7-08A22EB428F2}"/>
-    <hyperlink ref="B18" r:id="rId16" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/serialize-and-deserialize-binary-tree/ojquestion" xr:uid="{E037B5D2-708F-4C02-9CFE-1A1A063FDC6C}"/>
-    <hyperlink ref="B19" r:id="rId17" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/serialize-and-deserialize-n-ary-tree/ojquestion" xr:uid="{DBE963A5-3090-4772-9200-809B161A96BD}"/>
-    <hyperlink ref="B20" r:id="rId18" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/left-view-of-a-binarytree/ojquestion" xr:uid="{DFE991D6-3919-4B12-8C9D-C4CAE99F260D}"/>
-    <hyperlink ref="B21" r:id="rId19" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/right-view-of-a-binarytree/ojquestion" xr:uid="{8C9EB3F1-6C0F-44FD-8F75-3E3581ED59D6}"/>
-    <hyperlink ref="B22" r:id="rId20" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/width-of-a-binary-tree/ojquestion" xr:uid="{B603B53F-EEB0-443D-9F75-FE01052EFC18}"/>
-    <hyperlink ref="B23" r:id="rId21" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/vertical-order-traversal-of-a-binarytree/ojquestion" xr:uid="{23AC6476-9A22-42D8-AF6B-6871CB782111}"/>
-    <hyperlink ref="B24" r:id="rId22" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/vertical-order-traversal-of-a-binarytree-ii/ojquestion" xr:uid="{8F224D5E-DA14-4269-B26A-694253EC8DA0}"/>
-    <hyperlink ref="B25" r:id="rId23" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/bottom-view-of-a-binarytree/ojquestion" xr:uid="{BDDC2BBC-BB97-4552-AC6B-A450B82BB2EE}"/>
-    <hyperlink ref="B26" r:id="rId24" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/top-view-of-a-binarytree/ojquestion" xr:uid="{71B28E67-8AE9-423A-A53E-885DFAA6FD84}"/>
-    <hyperlink ref="B27" r:id="rId25" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/diagonal-order-of-a-binarytree/ojquestion" xr:uid="{2912C66C-8D98-42FE-AC40-59E4B98A0F5E}"/>
-    <hyperlink ref="B28" r:id="rId26" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/diagonal-order-(anti-clock-wise)-of-a-binarytree/ojquestion" xr:uid="{14E6AC0B-7B4D-49E3-8860-B0189EDF7E2B}"/>
-    <hyperlink ref="B29" r:id="rId27" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/vertical-order-sum-of-a-binarytree/ojquestion" xr:uid="{8D5E14C2-87A6-40F2-B6A2-E7C17DADF1E7}"/>
-    <hyperlink ref="B30" r:id="rId28" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/diagonal-order-sum-of-a-binary-tree/ojquestion" xr:uid="{1703CE23-3DEF-4994-9A7D-0604958F9773}"/>
-    <hyperlink ref="B31" r:id="rId29" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/bst-iterator/ojquestion" xr:uid="{EF5A17BA-00B5-43AD-9E53-33C4F38EC34A}"/>
-    <hyperlink ref="B32" r:id="rId30" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/node-to-root-path-binary-tree/ojquestion" xr:uid="{9929D7C8-6D2D-4EE9-9A9F-6E753B968476}"/>
-    <hyperlink ref="B33" r:id="rId31" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/all-single-child-parent-in-binary-tree/ojquestion" xr:uid="{D062EF98-5620-44D7-AAE3-581FF516B688}"/>
-    <hyperlink ref="B34" r:id="rId32" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/count-all-single-child-parent-in-binary-tree/ojquestion" xr:uid="{87EB2FB0-6CC4-4C40-826F-2FD9ED57A6C3}"/>
-    <hyperlink ref="B35" r:id="rId33" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/all-nodes-distance-k-in-binarytree/ojquestion" xr:uid="{BFF4672B-8432-4C62-9E99-0A85F5FC6197}"/>
-    <hyperlink ref="B36" r:id="rId34" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/burning-tree-/ojquestion" xr:uid="{10D86AE8-D0B2-41BE-ACE9-08C3CD6897ED}"/>
-    <hyperlink ref="B37" r:id="rId35" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/burning-tree-2/ojquestion" xr:uid="{207F8696-13B7-4080-A3A7-94C5832A75BA}"/>
-    <hyperlink ref="B38" r:id="rId36" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/maximum-width-of-binary-tree/ojquestion" xr:uid="{B3B28926-B4B3-4A0B-B2A0-106B1E3E6976}"/>
-    <hyperlink ref="B39" r:id="rId37" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/convert-binary-search-tree-to-doubly-linked-list/ojquestion" xr:uid="{209C430B-3FDB-47AB-B823-EAE30D572007}"/>
-    <hyperlink ref="B40" r:id="rId38" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/convert-sorted-dll-to-bst/ojquestion" xr:uid="{8A30E3D2-B223-43BA-90B5-23B1BA92321B}"/>
-    <hyperlink ref="B41" r:id="rId39" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/path-sum-in-binary-tree/ojquestion" xr:uid="{FB801C9E-A3DB-413E-A502-3D5C84BD4ABC}"/>
-    <hyperlink ref="B42" r:id="rId40" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/path-sum-in-binary-tree-2/ojquestion" xr:uid="{BBB40B81-B756-4927-9A69-A09A59EF1809}"/>
-    <hyperlink ref="B43" r:id="rId41" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/diameter-of-binary-tree-all-methods/ojquestion" xr:uid="{3BAB9480-BF54-4119-93A9-10564C6E77FF}"/>
-    <hyperlink ref="B44" r:id="rId42" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/maximum-path-sum-in-between-two-leaves-of-bt/ojquestion" xr:uid="{B16476BE-C6A7-42EC-900E-CEF358F23A0C}"/>
-    <hyperlink ref="B45" r:id="rId43" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/maximum-path-sum-of-binary-tree/ojquestion" xr:uid="{6B4C1CD4-2B23-41EF-AC8D-1BAA60DDFCD9}"/>
-    <hyperlink ref="B46" r:id="rId44" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/path-sum-equal-to-given-value/ojquestion" xr:uid="{4487FF04-8943-43A4-913B-B3107D43562F}"/>
-    <hyperlink ref="B47" r:id="rId45" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/lca-of-a-bt/ojquestion" xr:uid="{439A42DA-11D6-4F1C-90AB-7BDD9CB5E5BF}"/>
-    <hyperlink ref="B48" r:id="rId46" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/unique-binary-search-trees2-official/ojquestion" xr:uid="{F76311CC-32A5-4105-9530-AB35BF051349}"/>
-    <hyperlink ref="B49" r:id="rId47" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/all-possible-full-binary-trees-official/ojquestion" xr:uid="{ECCA5DA9-2616-41A1-BC52-F1C07A47D80C}"/>
-    <hyperlink ref="B50" r:id="rId48" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/add-one-row-to-tree-official/ojquestion" xr:uid="{B9CD03AF-8C3B-467E-A337-6833B934B499}"/>
-    <hyperlink ref="B51" r:id="rId49" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/path-in-zigzag-labelled-binary-tree-official/ojquestion" xr:uid="{84B77DD0-4AF0-455A-B2FB-DA296E847579}"/>
-    <hyperlink ref="B52" r:id="rId50" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/complete-binary-tree-inserter-official/ojquestion" xr:uid="{153801F5-3C1C-4201-B5C8-052E6858E31B}"/>
-    <hyperlink ref="B53" r:id="rId51" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/delete-nodes-and-return-forest-official/ojquestion" xr:uid="{00FBD558-BC0F-438B-A3FB-D52B9050FCC9}"/>
-    <hyperlink ref="B54" r:id="rId52" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/count-good-nodes-in-binary-tree-official/ojquestion" xr:uid="{9D0C2F63-F424-414D-80CF-4AB50C2AA5DD}"/>
-    <hyperlink ref="B55" r:id="rId53" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/even-odd-tree/ojquestion" xr:uid="{0FD2EE64-938F-4BC1-84E6-2DC4FA7307DB}"/>
-    <hyperlink ref="B56" r:id="rId54" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/longest-univalue-path/ojquestion" xr:uid="{519C2BAB-ACF3-4182-B0BB-EF3A4242B18B}"/>
-    <hyperlink ref="B57" r:id="rId55" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/populating-next-right-pointers-in-each-node/ojquestion" xr:uid="{C3FC6940-133D-4AE1-B7F2-CA99F316C91D}"/>
-    <hyperlink ref="B58" r:id="rId56" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/binary-tree-coloring-official/ojquestion" xr:uid="{EE1D8C5C-759C-4D1D-B4E9-1DEF9130BA1E}"/>
-    <hyperlink ref="B59" r:id="rId57" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/-find-a-corresponding-node-of-a-binary-tree-in-a-clone-of-that-tree/ojquestion" xr:uid="{E322B815-C741-4710-B7D8-495A84576D7D}"/>
+    <hyperlink ref="B3" r:id="rId1" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/coloring-a-border-official/ojquestion" xr:uid="{0A849A7B-76A7-471C-A059-C4CB7D7A7611}"/>
+    <hyperlink ref="B4" r:id="rId2" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/number-of-enclaves-official/ojquestion" xr:uid="{11B8D761-B301-4DBC-94B4-210275EB2B91}"/>
+    <hyperlink ref="B5" r:id="rId3" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/number-of-distinct-island-official/ojquestion" xr:uid="{C96DBBF5-BFF4-4A50-89F4-1EA48C4499BE}"/>
+    <hyperlink ref="B6" r:id="rId4" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/zero-one-matrix-official/ojquestion" xr:uid="{E178ED51-8C3B-4572-8EAB-13890E60E9B0}"/>
+    <hyperlink ref="B7" r:id="rId5" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/rotting-oranges-official/ojquestion" xr:uid="{A91A7A76-B4F5-44EC-863F-F3858BB96ACB}"/>
+    <hyperlink ref="B8" r:id="rId6" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/as-far-from-land-as-possible-official/ojquestion" xr:uid="{823DAFA4-7B72-44C9-8B10-A666F58F49EA}"/>
+    <hyperlink ref="B9" r:id="rId7" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/shortest-bridge-official/ojquestion" xr:uid="{D984F3DA-EF81-44C4-814D-7835D95C369C}"/>
+    <hyperlink ref="B10" r:id="rId8" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/bus-routes-official/ojquestion" xr:uid="{70B95DCF-6EA4-4DE2-AE0E-C9F2165446D7}"/>
+    <hyperlink ref="B11" r:id="rId9" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/sliding-puzzle-official/ojquestion" xr:uid="{9B5B87DC-7F61-4DA4-9EAA-4540919D4DA3}"/>
+    <hyperlink ref="B12" r:id="rId10" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/minimum-number-of-swaps-required-to-sort-an-array-official/ojquestion" xr:uid="{A6E082C4-9DE0-4445-838D-16EF79DED18F}"/>
+    <hyperlink ref="B13" r:id="rId11" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/pepcoder-and-reversing-official/ojquestion" xr:uid="{467C5D45-DF48-4ECB-8BBF-30813A56D3E5}"/>
+    <hyperlink ref="B14" r:id="rId12" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/pepcoding-course-schedule/ojquestion" xr:uid="{20F1A1CD-5B77-4C04-9325-6B5D845406F7}"/>
+    <hyperlink ref="B15" r:id="rId13" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/alien-dictionary-official/ojquestion" xr:uid="{32052FB7-D6D5-4623-B582-429BFA56162E}"/>
+    <hyperlink ref="B16" r:id="rId14" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/kruskal-algorithm-official/ojquestion" xr:uid="{140122C9-8888-486D-8769-42D20988E3DD}"/>
+    <hyperlink ref="B17" r:id="rId15" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/optimize-water-distribution-official/ojquestion" xr:uid="{77069B0F-34B4-44FA-9ADD-A95A38D842D0}"/>
+    <hyperlink ref="B18" r:id="rId16" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/swim-in-rising-water-official/ojquestion" xr:uid="{58572896-4199-4D10-9D0C-9B2B0EFCE8FD}"/>
+    <hyperlink ref="B19" r:id="rId17" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/minimum-cost-to-connect-all-cities-official/ojquestion" xr:uid="{3FBA94BC-2223-4A3A-9860-268407706F16}"/>
+    <hyperlink ref="B20" r:id="rId18" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/bellman-ford-official/ojquestion" xr:uid="{076D714F-E7E1-45DB-A59C-E7BD78BD00EC}"/>
+    <hyperlink ref="B21" r:id="rId19" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/negative-weight-cycle-official/ojquestion" xr:uid="{7F85F52B-723E-4045-8262-4FE764C37B13}"/>
+    <hyperlink ref="B22" r:id="rId20" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/kosaraju-algorithm-official/ojquestion" xr:uid="{DA330B95-50EC-4E4A-B54E-3AC48083E411}"/>
+    <hyperlink ref="B23" r:id="rId21" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/mother-vertex-official/ojquestion" xr:uid="{662CE2A4-18D9-4AFD-A0EC-2B988C71BD09}"/>
+    <hyperlink ref="B24" r:id="rId22" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/articulation-point-official/ojquestion" xr:uid="{AF8A7C3D-48C4-470C-9197-ABAF354CECFE}"/>
+    <hyperlink ref="B25" r:id="rId23" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/critical-connection-official/ojquestion" xr:uid="{ABEB382C-2F4E-400C-BFDB-2A76D27D8257}"/>
+    <hyperlink ref="B26" r:id="rId24" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/remove-max-number-of-edges-to-keep-graph-fully-traversable-official/ojquestion" xr:uid="{1CD65075-BBCD-4067-A799-3B1E0248273A}"/>
+    <hyperlink ref="B27" r:id="rId25" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/number-of-island-2-official/ojquestion" xr:uid="{99751C73-6FDA-4517-8491-F2717C86D5EC}"/>
+    <hyperlink ref="B28" r:id="rId26" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/regions-cut-by-slashes-official/ojquestion" xr:uid="{C4239AC2-9246-42D9-871B-4FE66A92AA3C}"/>
+    <hyperlink ref="B29" r:id="rId27" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/reconstruct-itinerary-official/ojquestion" xr:uid="{1F131268-2AAF-4340-A5FA-1E763C5505AF}"/>
+    <hyperlink ref="B30" r:id="rId28" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/rank--transform-of-a-matrix-official/ojquestion" xr:uid="{BB1869BD-B70D-4841-BEE1-E2E5ACCABB83}"/>
+    <hyperlink ref="B31" r:id="rId29" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/accounts-merge-official/ojquestion" xr:uid="{68EC6C69-9B70-4A28-9AE8-44D82F3A492C}"/>
+    <hyperlink ref="B32" r:id="rId30" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/minimize-malware-spread-official/ojquestion" xr:uid="{CA1E5FED-BF27-4AE8-82AE-B3785BFD6764}"/>
+    <hyperlink ref="B33" r:id="rId31" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/minimize-malware-spread-ii-official/ojquestion" xr:uid="{2784F6E3-7EC9-44A2-BA40-9E5E2F5A3CE9}"/>
+    <hyperlink ref="B34" r:id="rId32" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/redundant-connection-official/ojquestion" xr:uid="{9A01354F-423D-41F9-AA6B-8CBFCCDCC7BF}"/>
+    <hyperlink ref="B35" r:id="rId33" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/minimize-hamming--distance-after-swap-operations-official/ojquestion" xr:uid="{A9A908F8-0AB7-4BA2-8F4C-257BEB8291EA}"/>
+    <hyperlink ref="B36" r:id="rId34" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/redundant-connection-2-official/ojquestion" xr:uid="{7AB95D1E-4D3C-4016-9945-052E9F292CF0}"/>
+    <hyperlink ref="B37" r:id="rId35" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/satisfiability-of-equality-equation-official/ojquestion" xr:uid="{3A55514E-91AF-4489-9F0D-6B1D1E568F99}"/>
+    <hyperlink ref="B38" r:id="rId36" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/sentence_similarity_official/ojquestion" xr:uid="{955873BF-E5D9-484B-AA53-AD1D62AF8DFB}"/>
+    <hyperlink ref="B39" r:id="rId37" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/park-regions-official/ojquestion" xr:uid="{B22E6F5A-50C2-427C-A986-7AB112B8420C}"/>
+    <hyperlink ref="B40" r:id="rId38" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/kill-the-most-monsters/ojquestion" xr:uid="{4A25245F-FDC0-429A-A2E2-96B6FF4699AA}"/>
+    <hyperlink ref="B41" r:id="rId39" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/number-of-connections-to-make-pipeline-connected/ojquestion" xr:uid="{80DC846C-B2CD-4BEB-8448-A70928659A62}"/>
+    <hyperlink ref="B42" r:id="rId40" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/number-of-provinces/ojquestion" xr:uid="{7B30F223-F927-4C1E-A94B-014ECEE97A50}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5137,8 +5204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A2:B67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B67"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5539,86 +5606,137 @@
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>49</v>
+      </c>
       <c r="B51" s="2" t="s">
         <v>393</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>50</v>
+      </c>
       <c r="B52" s="2" t="s">
         <v>394</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>51</v>
+      </c>
       <c r="B53" s="2" t="s">
         <v>395</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>52</v>
+      </c>
       <c r="B54" s="2" t="s">
         <v>396</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>53</v>
+      </c>
       <c r="B55" s="2" t="s">
         <v>397</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>54</v>
+      </c>
       <c r="B56" s="2" t="s">
         <v>398</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>55</v>
+      </c>
       <c r="B57" s="2" t="s">
         <v>399</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>56</v>
+      </c>
       <c r="B58" s="2" t="s">
         <v>400</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>57</v>
+      </c>
       <c r="B59" s="2" t="s">
         <v>401</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>58</v>
+      </c>
       <c r="B60" s="2" t="s">
         <v>402</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>59</v>
+      </c>
       <c r="B61" s="2" t="s">
         <v>403</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>60</v>
+      </c>
       <c r="B62" s="2" t="s">
         <v>404</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>61</v>
+      </c>
       <c r="B63" s="2" t="s">
         <v>405</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>62</v>
+      </c>
       <c r="B64" s="2" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>63</v>
+      </c>
       <c r="B65" s="2" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>64</v>
+      </c>
       <c r="B66" s="2" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>65</v>
+      </c>
       <c r="B67" s="2" t="s">
         <v>409</v>
       </c>
@@ -5696,16 +5814,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A2:B42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A2:C59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B42"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="43.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -5721,7 +5839,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>361</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -5729,7 +5847,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>151</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -5737,7 +5855,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -5745,7 +5863,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -5753,7 +5871,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>362</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -5761,7 +5879,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>363</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -5769,7 +5887,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>364</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -5777,7 +5895,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>365</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -5785,15 +5903,15 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>367</v>
+        <v>410</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -5801,599 +5919,455 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>146</v>
+        <v>411</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>12</v>
+      </c>
       <c r="B14" s="2" t="s">
-        <v>147</v>
+        <v>161</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>13</v>
+      </c>
       <c r="B15" s="2" t="s">
-        <v>368</v>
+        <v>162</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>14</v>
+      </c>
       <c r="B16" s="2" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>15</v>
+      </c>
       <c r="B17" s="2" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>16</v>
+      </c>
       <c r="B18" s="2" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>17</v>
+      </c>
       <c r="B19" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>18</v>
+      </c>
       <c r="B20" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>19</v>
+      </c>
       <c r="B21" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>20</v>
+      </c>
       <c r="B22" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>21</v>
+      </c>
       <c r="B23" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>22</v>
+      </c>
       <c r="B24" s="2" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>23</v>
+      </c>
       <c r="B25" s="2" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="26" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>24</v>
+      </c>
       <c r="B26" s="2" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>25</v>
+      </c>
       <c r="B27" s="2" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>26</v>
+      </c>
       <c r="B28" s="2" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>27</v>
+      </c>
       <c r="B29" s="2" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>28</v>
+      </c>
       <c r="B30" s="2" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>29</v>
+      </c>
       <c r="B31" s="2" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>30</v>
+      </c>
       <c r="B32" s="2" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>31</v>
+      </c>
       <c r="B33" s="2" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>32</v>
+      </c>
       <c r="B34" s="2" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>33</v>
+      </c>
       <c r="B35" s="2" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>34</v>
+      </c>
       <c r="B36" s="2" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>35</v>
+      </c>
       <c r="B37" s="2" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>36</v>
+      </c>
       <c r="B38" s="2" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>37</v>
+      </c>
       <c r="B39" s="2" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>38</v>
+      </c>
       <c r="B40" s="2" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="41" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>39</v>
+      </c>
       <c r="B41" s="2" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>40</v>
+      </c>
       <c r="B42" s="2" t="s">
-        <v>390</v>
+        <v>420</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="C43" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>42</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="C44" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="C45" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>44</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>45</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>46</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>47</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>48</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>49</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>50</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>51</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>52</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>53</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>54</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>55</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>56</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>57</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>437</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/coloring-a-border-official/ojquestion" xr:uid="{0A849A7B-76A7-471C-A059-C4CB7D7A7611}"/>
-    <hyperlink ref="B4" r:id="rId2" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/number-of-enclaves-official/ojquestion" xr:uid="{11B8D761-B301-4DBC-94B4-210275EB2B91}"/>
-    <hyperlink ref="B5" r:id="rId3" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/number-of-distinct-island-official/ojquestion" xr:uid="{C96DBBF5-BFF4-4A50-89F4-1EA48C4499BE}"/>
-    <hyperlink ref="B6" r:id="rId4" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/zero-one-matrix-official/ojquestion" xr:uid="{E178ED51-8C3B-4572-8EAB-13890E60E9B0}"/>
-    <hyperlink ref="B7" r:id="rId5" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/rotting-oranges-official/ojquestion" xr:uid="{A91A7A76-B4F5-44EC-863F-F3858BB96ACB}"/>
-    <hyperlink ref="B8" r:id="rId6" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/as-far-from-land-as-possible-official/ojquestion" xr:uid="{823DAFA4-7B72-44C9-8B10-A666F58F49EA}"/>
-    <hyperlink ref="B9" r:id="rId7" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/shortest-bridge-official/ojquestion" xr:uid="{D984F3DA-EF81-44C4-814D-7835D95C369C}"/>
-    <hyperlink ref="B10" r:id="rId8" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/bus-routes-official/ojquestion" xr:uid="{70B95DCF-6EA4-4DE2-AE0E-C9F2165446D7}"/>
-    <hyperlink ref="B11" r:id="rId9" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/sliding-puzzle-official/ojquestion" xr:uid="{9B5B87DC-7F61-4DA4-9EAA-4540919D4DA3}"/>
-    <hyperlink ref="B12" r:id="rId10" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/minimum-number-of-swaps-required-to-sort-an-array-official/ojquestion" xr:uid="{A6E082C4-9DE0-4445-838D-16EF79DED18F}"/>
-    <hyperlink ref="B13" r:id="rId11" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/pepcoder-and-reversing-official/ojquestion" xr:uid="{467C5D45-DF48-4ECB-8BBF-30813A56D3E5}"/>
-    <hyperlink ref="B14" r:id="rId12" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/pepcoding-course-schedule/ojquestion" xr:uid="{20F1A1CD-5B77-4C04-9325-6B5D845406F7}"/>
-    <hyperlink ref="B15" r:id="rId13" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/alien-dictionary-official/ojquestion" xr:uid="{32052FB7-D6D5-4623-B582-429BFA56162E}"/>
-    <hyperlink ref="B16" r:id="rId14" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/kruskal-algorithm-official/ojquestion" xr:uid="{140122C9-8888-486D-8769-42D20988E3DD}"/>
-    <hyperlink ref="B17" r:id="rId15" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/optimize-water-distribution-official/ojquestion" xr:uid="{77069B0F-34B4-44FA-9ADD-A95A38D842D0}"/>
-    <hyperlink ref="B18" r:id="rId16" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/swim-in-rising-water-official/ojquestion" xr:uid="{58572896-4199-4D10-9D0C-9B2B0EFCE8FD}"/>
-    <hyperlink ref="B19" r:id="rId17" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/minimum-cost-to-connect-all-cities-official/ojquestion" xr:uid="{3FBA94BC-2223-4A3A-9860-268407706F16}"/>
-    <hyperlink ref="B20" r:id="rId18" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/bellman-ford-official/ojquestion" xr:uid="{076D714F-E7E1-45DB-A59C-E7BD78BD00EC}"/>
-    <hyperlink ref="B21" r:id="rId19" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/negative-weight-cycle-official/ojquestion" xr:uid="{7F85F52B-723E-4045-8262-4FE764C37B13}"/>
-    <hyperlink ref="B22" r:id="rId20" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/kosaraju-algorithm-official/ojquestion" xr:uid="{DA330B95-50EC-4E4A-B54E-3AC48083E411}"/>
-    <hyperlink ref="B23" r:id="rId21" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/mother-vertex-official/ojquestion" xr:uid="{662CE2A4-18D9-4AFD-A0EC-2B988C71BD09}"/>
-    <hyperlink ref="B24" r:id="rId22" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/articulation-point-official/ojquestion" xr:uid="{AF8A7C3D-48C4-470C-9197-ABAF354CECFE}"/>
-    <hyperlink ref="B25" r:id="rId23" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/critical-connection-official/ojquestion" xr:uid="{ABEB382C-2F4E-400C-BFDB-2A76D27D8257}"/>
-    <hyperlink ref="B26" r:id="rId24" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/remove-max-number-of-edges-to-keep-graph-fully-traversable-official/ojquestion" xr:uid="{1CD65075-BBCD-4067-A799-3B1E0248273A}"/>
-    <hyperlink ref="B27" r:id="rId25" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/number-of-island-2-official/ojquestion" xr:uid="{99751C73-6FDA-4517-8491-F2717C86D5EC}"/>
-    <hyperlink ref="B28" r:id="rId26" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/regions-cut-by-slashes-official/ojquestion" xr:uid="{C4239AC2-9246-42D9-871B-4FE66A92AA3C}"/>
-    <hyperlink ref="B29" r:id="rId27" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/reconstruct-itinerary-official/ojquestion" xr:uid="{1F131268-2AAF-4340-A5FA-1E763C5505AF}"/>
-    <hyperlink ref="B30" r:id="rId28" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/rank--transform-of-a-matrix-official/ojquestion" xr:uid="{BB1869BD-B70D-4841-BEE1-E2E5ACCABB83}"/>
-    <hyperlink ref="B31" r:id="rId29" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/accounts-merge-official/ojquestion" xr:uid="{68EC6C69-9B70-4A28-9AE8-44D82F3A492C}"/>
-    <hyperlink ref="B32" r:id="rId30" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/minimize-malware-spread-official/ojquestion" xr:uid="{CA1E5FED-BF27-4AE8-82AE-B3785BFD6764}"/>
-    <hyperlink ref="B33" r:id="rId31" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/minimize-malware-spread-ii-official/ojquestion" xr:uid="{2784F6E3-7EC9-44A2-BA40-9E5E2F5A3CE9}"/>
-    <hyperlink ref="B34" r:id="rId32" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/redundant-connection-official/ojquestion" xr:uid="{9A01354F-423D-41F9-AA6B-8CBFCCDCC7BF}"/>
-    <hyperlink ref="B35" r:id="rId33" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/minimize-hamming--distance-after-swap-operations-official/ojquestion" xr:uid="{A9A908F8-0AB7-4BA2-8F4C-257BEB8291EA}"/>
-    <hyperlink ref="B36" r:id="rId34" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/redundant-connection-2-official/ojquestion" xr:uid="{7AB95D1E-4D3C-4016-9945-052E9F292CF0}"/>
-    <hyperlink ref="B37" r:id="rId35" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/satisfiability-of-equality-equation-official/ojquestion" xr:uid="{3A55514E-91AF-4489-9F0D-6B1D1E568F99}"/>
-    <hyperlink ref="B38" r:id="rId36" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/sentence_similarity_official/ojquestion" xr:uid="{955873BF-E5D9-484B-AA53-AD1D62AF8DFB}"/>
-    <hyperlink ref="B39" r:id="rId37" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/park-regions-official/ojquestion" xr:uid="{B22E6F5A-50C2-427C-A986-7AB112B8420C}"/>
-    <hyperlink ref="B40" r:id="rId38" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/kill-the-most-monsters/ojquestion" xr:uid="{4A25245F-FDC0-429A-A2E2-96B6FF4699AA}"/>
-    <hyperlink ref="B41" r:id="rId39" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/number-of-connections-to-make-pipeline-connected/ojquestion" xr:uid="{80DC846C-B2CD-4BEB-8448-A70928659A62}"/>
-    <hyperlink ref="B42" r:id="rId40" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/number-of-provinces/ojquestion" xr:uid="{7B30F223-F927-4C1E-A94B-014ECEE97A50}"/>
+    <hyperlink ref="B3" r:id="rId1" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/in-order-morris-traversal-in-binarytree/ojquestion" xr:uid="{12FE414D-86EC-4703-89B8-46439B34D434}"/>
+    <hyperlink ref="B4" r:id="rId2" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/pre-order-morris-traversal-in-binary-tree/ojquestion" xr:uid="{08B75074-0749-4158-B777-D7C28A447CDD}"/>
+    <hyperlink ref="B5" r:id="rId3" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/cameras-in-binary-tree-official/ojquestion" xr:uid="{766A30BC-D241-4F59-9799-3F802861EFA8}"/>
+    <hyperlink ref="B6" r:id="rId4" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/levelup_house-robber-in-binary-tree/ojquestion" xr:uid="{5006CB72-6882-4AF8-B797-ECC3B3688491}"/>
+    <hyperlink ref="B7" r:id="rId5" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/longest-zigzag-path-in-a-binary-tree/ojquestion" xr:uid="{71FF4B48-68F7-4A31-9152-1A98444F8F1C}"/>
+    <hyperlink ref="B8" r:id="rId6" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/levelup_validate-bst/ojquestion" xr:uid="{2376104C-A4E1-4B92-A733-4EE741230FC5}"/>
+    <hyperlink ref="B9" r:id="rId7" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/recover-bst/ojquestion" xr:uid="{BA60A109-AAF7-4998-BBA5-13BCB53EDC8D}"/>
+    <hyperlink ref="B10" r:id="rId8" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/construct-binarytree-from-preorder-and-inorder-traversal/ojquestion" xr:uid="{36463C2E-5A17-437B-865D-4051FDD5C52E}"/>
+    <hyperlink ref="B11" r:id="rId9" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/construct-binarytree-from-postorder-and-inorder-traversal/ojquestion" xr:uid="{936FAD46-6EB8-4AB6-9CA8-AA7BCE58678D}"/>
+    <hyperlink ref="B12" r:id="rId10" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/construct-binarytree-from-inorder-and-levelorder-traversal/ojquestion" xr:uid="{12969EDF-DA52-4F3B-A353-43B0D8E2AD8C}"/>
+    <hyperlink ref="B13" r:id="rId11" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/construct-binary-tree-from-levelorder-and-inorder-traversal/ojquestion" xr:uid="{AFEF680C-5099-489D-8DE5-D926E37189F5}"/>
+    <hyperlink ref="B14" r:id="rId12" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/construct-bst-from-inorder-traversal/ojquestion" xr:uid="{C7E3583C-89E4-4578-AD50-49378E673B2D}"/>
+    <hyperlink ref="B15" r:id="rId13" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/construct-bst-from-preorder-traversal/ojquestion" xr:uid="{70A85115-3368-4BDB-BEF6-5D7CA73E256A}"/>
+    <hyperlink ref="B16" r:id="rId14" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/construct-bst-from-postorder-traversal/ojquestion" xr:uid="{232E7B35-A67D-4094-AED1-925211E5CE54}"/>
+    <hyperlink ref="B17" r:id="rId15" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/construct-bst-from-levelorder-traversal/ojquestion" xr:uid="{42913B87-06BD-4CC0-98B7-08A22EB428F2}"/>
+    <hyperlink ref="B18" r:id="rId16" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/serialize-and-deserialize-binary-tree/ojquestion" xr:uid="{E037B5D2-708F-4C02-9CFE-1A1A063FDC6C}"/>
+    <hyperlink ref="B19" r:id="rId17" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/serialize-and-deserialize-n-ary-tree/ojquestion" xr:uid="{DBE963A5-3090-4772-9200-809B161A96BD}"/>
+    <hyperlink ref="B20" r:id="rId18" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/left-view-of-a-binarytree/ojquestion" xr:uid="{DFE991D6-3919-4B12-8C9D-C4CAE99F260D}"/>
+    <hyperlink ref="B21" r:id="rId19" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/right-view-of-a-binarytree/ojquestion" xr:uid="{8C9EB3F1-6C0F-44FD-8F75-3E3581ED59D6}"/>
+    <hyperlink ref="B22" r:id="rId20" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/width-of-a-binary-tree/ojquestion" xr:uid="{B603B53F-EEB0-443D-9F75-FE01052EFC18}"/>
+    <hyperlink ref="B23" r:id="rId21" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/vertical-order-traversal-of-a-binarytree/ojquestion" xr:uid="{23AC6476-9A22-42D8-AF6B-6871CB782111}"/>
+    <hyperlink ref="B24" r:id="rId22" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/vertical-order-traversal-of-a-binarytree-ii/ojquestion" xr:uid="{8F224D5E-DA14-4269-B26A-694253EC8DA0}"/>
+    <hyperlink ref="B25" r:id="rId23" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/bottom-view-of-a-binarytree/ojquestion" xr:uid="{BDDC2BBC-BB97-4552-AC6B-A450B82BB2EE}"/>
+    <hyperlink ref="B26" r:id="rId24" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/top-view-of-a-binarytree/ojquestion" xr:uid="{71B28E67-8AE9-423A-A53E-885DFAA6FD84}"/>
+    <hyperlink ref="B27" r:id="rId25" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/diagonal-order-of-a-binarytree/ojquestion" xr:uid="{2912C66C-8D98-42FE-AC40-59E4B98A0F5E}"/>
+    <hyperlink ref="B28" r:id="rId26" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/diagonal-order-(anti-clock-wise)-of-a-binarytree/ojquestion" xr:uid="{14E6AC0B-7B4D-49E3-8860-B0189EDF7E2B}"/>
+    <hyperlink ref="B29" r:id="rId27" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/vertical-order-sum-of-a-binarytree/ojquestion" xr:uid="{8D5E14C2-87A6-40F2-B6A2-E7C17DADF1E7}"/>
+    <hyperlink ref="B30" r:id="rId28" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/diagonal-order-sum-of-a-binary-tree/ojquestion" xr:uid="{1703CE23-3DEF-4994-9A7D-0604958F9773}"/>
+    <hyperlink ref="B31" r:id="rId29" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/bst-iterator/ojquestion" xr:uid="{EF5A17BA-00B5-43AD-9E53-33C4F38EC34A}"/>
+    <hyperlink ref="B32" r:id="rId30" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/node-to-root-path-binary-tree/ojquestion" xr:uid="{9929D7C8-6D2D-4EE9-9A9F-6E753B968476}"/>
+    <hyperlink ref="B33" r:id="rId31" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/all-single-child-parent-in-binary-tree/ojquestion" xr:uid="{D062EF98-5620-44D7-AAE3-581FF516B688}"/>
+    <hyperlink ref="B34" r:id="rId32" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/count-all-single-child-parent-in-binary-tree/ojquestion" xr:uid="{87EB2FB0-6CC4-4C40-826F-2FD9ED57A6C3}"/>
+    <hyperlink ref="B35" r:id="rId33" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/all-nodes-distance-k-in-binarytree/ojquestion" xr:uid="{BFF4672B-8432-4C62-9E99-0A85F5FC6197}"/>
+    <hyperlink ref="B36" r:id="rId34" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/burning-tree-/ojquestion" xr:uid="{10D86AE8-D0B2-41BE-ACE9-08C3CD6897ED}"/>
+    <hyperlink ref="B37" r:id="rId35" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/burning-tree-2/ojquestion" xr:uid="{207F8696-13B7-4080-A3A7-94C5832A75BA}"/>
+    <hyperlink ref="B38" r:id="rId36" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/maximum-width-of-binary-tree/ojquestion" xr:uid="{B3B28926-B4B3-4A0B-B2A0-106B1E3E6976}"/>
+    <hyperlink ref="B39" r:id="rId37" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/convert-binary-search-tree-to-doubly-linked-list/ojquestion" xr:uid="{209C430B-3FDB-47AB-B823-EAE30D572007}"/>
+    <hyperlink ref="B40" r:id="rId38" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/convert-sorted-dll-to-bst/ojquestion" xr:uid="{8A30E3D2-B223-43BA-90B5-23B1BA92321B}"/>
+    <hyperlink ref="B41" r:id="rId39" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/path-sum-in-binary-tree/ojquestion" xr:uid="{FB801C9E-A3DB-413E-A502-3D5C84BD4ABC}"/>
+    <hyperlink ref="B42" r:id="rId40" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/path-sum-in-binary-tree-2/ojquestion" xr:uid="{BBB40B81-B756-4927-9A69-A09A59EF1809}"/>
+    <hyperlink ref="B43" r:id="rId41" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/diameter-of-binary-tree-all-methods/ojquestion" xr:uid="{3BAB9480-BF54-4119-93A9-10564C6E77FF}"/>
+    <hyperlink ref="B44" r:id="rId42" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/maximum-path-sum-in-between-two-leaves-of-bt/ojquestion" xr:uid="{B16476BE-C6A7-42EC-900E-CEF358F23A0C}"/>
+    <hyperlink ref="B45" r:id="rId43" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/maximum-path-sum-of-binary-tree/ojquestion" xr:uid="{6B4C1CD4-2B23-41EF-AC8D-1BAA60DDFCD9}"/>
+    <hyperlink ref="B46" r:id="rId44" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/path-sum-equal-to-given-value/ojquestion" xr:uid="{4487FF04-8943-43A4-913B-B3107D43562F}"/>
+    <hyperlink ref="B47" r:id="rId45" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/lca-of-a-bt/ojquestion" xr:uid="{439A42DA-11D6-4F1C-90AB-7BDD9CB5E5BF}"/>
+    <hyperlink ref="B48" r:id="rId46" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/unique-binary-search-trees2-official/ojquestion" xr:uid="{F76311CC-32A5-4105-9530-AB35BF051349}"/>
+    <hyperlink ref="B49" r:id="rId47" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/all-possible-full-binary-trees-official/ojquestion" xr:uid="{ECCA5DA9-2616-41A1-BC52-F1C07A47D80C}"/>
+    <hyperlink ref="B50" r:id="rId48" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/add-one-row-to-tree-official/ojquestion" xr:uid="{B9CD03AF-8C3B-467E-A337-6833B934B499}"/>
+    <hyperlink ref="B51" r:id="rId49" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/path-in-zigzag-labelled-binary-tree-official/ojquestion" xr:uid="{84B77DD0-4AF0-455A-B2FB-DA296E847579}"/>
+    <hyperlink ref="B52" r:id="rId50" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/complete-binary-tree-inserter-official/ojquestion" xr:uid="{153801F5-3C1C-4201-B5C8-052E6858E31B}"/>
+    <hyperlink ref="B53" r:id="rId51" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/delete-nodes-and-return-forest-official/ojquestion" xr:uid="{00FBD558-BC0F-438B-A3FB-D52B9050FCC9}"/>
+    <hyperlink ref="B54" r:id="rId52" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/count-good-nodes-in-binary-tree-official/ojquestion" xr:uid="{9D0C2F63-F424-414D-80CF-4AB50C2AA5DD}"/>
+    <hyperlink ref="B55" r:id="rId53" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/even-odd-tree/ojquestion" xr:uid="{0FD2EE64-938F-4BC1-84E6-2DC4FA7307DB}"/>
+    <hyperlink ref="B56" r:id="rId54" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/longest-univalue-path/ojquestion" xr:uid="{519C2BAB-ACF3-4182-B0BB-EF3A4242B18B}"/>
+    <hyperlink ref="B57" r:id="rId55" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/populating-next-right-pointers-in-each-node/ojquestion" xr:uid="{C3FC6940-133D-4AE1-B7F2-CA99F316C91D}"/>
+    <hyperlink ref="B58" r:id="rId56" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/binary-tree-coloring-official/ojquestion" xr:uid="{EE1D8C5C-759C-4D1D-B4E9-1DEF9130BA1E}"/>
+    <hyperlink ref="B59" r:id="rId57" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/-find-a-corresponding-node-of-a-binary-tree-in-a-clone-of-that-tree/ojquestion" xr:uid="{E322B815-C741-4710-B7D8-495A84576D7D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A2:B36"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B36"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="59.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>12</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>13</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>14</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>15</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>16</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>17</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>18</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>19</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>20</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <v>21</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <v>22</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>23</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>24</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <v>25</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28">
-        <v>26</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29">
-        <v>27</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30">
-        <v>28</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B31" s="2" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B32" s="2" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B33" s="2" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B34" s="2" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B35" s="2" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B36" s="2" t="s">
-        <v>449</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/next-greater-element-official/ojquestion" xr:uid="{87FD3A23-B754-4247-819F-A63188639CAB}"/>
-    <hyperlink ref="B4" r:id="rId2" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/next-greater-element-left-official/ojquestion" xr:uid="{4180CC0D-6E46-412B-BB97-6F2C7B4D26C0}"/>
-    <hyperlink ref="B5" r:id="rId3" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/next-smaller-element-right-official/ojquestion" xr:uid="{001DDE2A-7B58-4272-88A1-B95092871A34}"/>
-    <hyperlink ref="B6" r:id="rId4" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/next-smaller-element-left-official/ojquestion" xr:uid="{BEAE2BA3-7C9E-4932-B25D-08716B524F10}"/>
-    <hyperlink ref="B7" r:id="rId5" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/next-greater-element-i-official/ojquestion" xr:uid="{5AA31017-3B6C-4190-8239-436BF115A0EA}"/>
-    <hyperlink ref="B8" r:id="rId6" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/next-greater-element-ii-official/ojquestion" xr:uid="{261A595A-9D7C-4369-8418-C2215270A8B8}"/>
-    <hyperlink ref="B9" r:id="rId7" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/largest-area-histogram2-official/ojquestion" xr:uid="{24BBC891-389D-4072-9833-330F9114F269}"/>
-    <hyperlink ref="B10" r:id="rId8" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/maximal-rectangle-official/ojquestion" xr:uid="{64BE7829-27B7-48E4-BA4F-3053A67E1D41}"/>
-    <hyperlink ref="B11" r:id="rId9" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/validate-stack-sequences-official/ojquestion" xr:uid="{688A8C49-2C09-4FAA-B6DC-552A42BF9F9C}"/>
-    <hyperlink ref="B12" r:id="rId10" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/minimum-add-to-make-parentheses-valid-official/ojquestion" xr:uid="{36F6B88B-8DAB-4A01-9D3C-3BADAB479ADB}"/>
-    <hyperlink ref="B13" r:id="rId11" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/remove-outermost-parentheses-official/ojquestion" xr:uid="{4B7845E4-D49A-46D7-BF18-D7409093AD19}"/>
-    <hyperlink ref="B14" r:id="rId12" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/score-of-parentheses-official/ojquestion" xr:uid="{799C5857-1C6B-45FE-8B3A-CAB7C071064B}"/>
-    <hyperlink ref="B15" r:id="rId13" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/reverse-substrings-between-each-pair-of-parentheses-official/ojquestion" xr:uid="{84954448-78C4-4779-839A-43C6CFD7E8F5}"/>
-    <hyperlink ref="B16" r:id="rId14" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/minimum-remove-to-make-valid-parentheses-official/ojquestion" xr:uid="{24507EBF-217F-4FCB-9961-05E8B5A039AF}"/>
-    <hyperlink ref="B17" r:id="rId15" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/online-stock-span-official/ojquestion" xr:uid="{C1711090-7144-46A8-B1D0-E53A3C2EDC1C}"/>
-    <hyperlink ref="B18" r:id="rId16" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/exclusive-time-of-functions-official/ojquestion" xr:uid="{7999D559-34C6-4528-BC05-8898761019C9}"/>
-    <hyperlink ref="B19" r:id="rId17" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/132-pattern-official/ojquestion" xr:uid="{1E571A53-F7D6-4121-9C21-E80CF9AA2778}"/>
-    <hyperlink ref="B20" r:id="rId18" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/asteroid-collision-official/ojquestion" xr:uid="{8F35580B-CD96-4B9B-AF5D-F023C77E9C1F}"/>
-    <hyperlink ref="B21" r:id="rId19" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/remove-k-digits-official/ojquestion" xr:uid="{970FEBE9-0716-4924-9CC2-DFB517E9505E}"/>
-    <hyperlink ref="B22" r:id="rId20" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/remove-duplicate-letters-official/ojquestion" xr:uid="{E42F647E-598B-4580-B5E3-FBA3BDA28062}"/>
-    <hyperlink ref="B23" r:id="rId21" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/trapping-rain-water-official/ojquestion" xr:uid="{27B26838-677E-4D04-9B2C-CB7598170412}"/>
-    <hyperlink ref="B24" r:id="rId22" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/trapping-rain-water-2-official/ojquestion" xr:uid="{9DA3D799-D2F1-4C20-8371-1931B67ECCD8}"/>
-    <hyperlink ref="B25" r:id="rId23" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/number-of-valid-subarrays-official/ojquestion" xr:uid="{464B85CF-3640-48AA-94D4-23D9DA08BBC2}"/>
-    <hyperlink ref="B26" r:id="rId24" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/basic-calculator-official/ojquestion" xr:uid="{1D423A5D-76BF-474D-B4BA-F118B4A791E5}"/>
-    <hyperlink ref="B27" r:id="rId25" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/basic-calculator-ii-official/ojquestion" xr:uid="{2DE15C8F-F385-4DA9-BB08-2405F0094362}"/>
-    <hyperlink ref="B28" r:id="rId26" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/basic-calculator-3-official/ojquestion" xr:uid="{AC707DA2-E4E2-488F-8EC8-181D87D0CE67}"/>
-    <hyperlink ref="B29" r:id="rId27" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/lexicographically-smallest-subsequence-official/ojquestion" xr:uid="{F8DCA947-F3F9-44F9-B656-16E9B0DB5FA3}"/>
-    <hyperlink ref="B30" r:id="rId28" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/design-a-stack-with-increment-operation-official/ojquestion" xr:uid="{056ADEE0-3A3A-4229-B514-75331785371F}"/>
-    <hyperlink ref="B31" r:id="rId29" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/design-circular-deque-official/ojquestion" xr:uid="{371CDA0B-CB92-4C7D-8C6D-262DE7F40094}"/>
-    <hyperlink ref="B32" r:id="rId30" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/max-stack-offical/ojquestion" xr:uid="{FE84D6E4-6D90-4281-A3C6-6B06A04B568E}"/>
-    <hyperlink ref="B33" r:id="rId31" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/check-if-word-is-valid-after-insertion-official/ojquestion" xr:uid="{FBFF2BF1-EE8F-401B-86F2-E146531BD60D}"/>
-    <hyperlink ref="B34" r:id="rId32" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/design-hit-counter-official/ojquestion" xr:uid="{F92DA8A1-3F95-49E9-BFDE-21291D10A370}"/>
-    <hyperlink ref="B35" r:id="rId33" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/number-of-recent-calls-official/ojquestion" xr:uid="{2A60B4A3-5175-478F-9920-6AB7A1E63DA1}"/>
-    <hyperlink ref="B36" r:id="rId34" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/moving-average-from-data-stream-official/ojquestion" xr:uid="{F1F3F1B5-B540-484F-BFE4-5896D6A32CAC}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC154703-7ACF-4C58-B783-B9BD29D8F343}">
-  <dimension ref="B2:B11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B4" s="1" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B5" s="1" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B6" s="1" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B7" s="1" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B8" s="1" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B9" s="1" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B10" s="1" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B11" s="1" t="s">
-        <v>459</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trie/implement-trie-official/ojquestion" xr:uid="{4764CADD-C9D7-44A8-9D88-33FF0FA050A7}"/>
-    <hyperlink ref="B3" r:id="rId2" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trie/design-add-and-search-words-data-structure-official/ojquestion" xr:uid="{98FFE7DE-3355-4C30-9D2F-20ECB21881D7}"/>
-    <hyperlink ref="B4" r:id="rId3" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trie/word-search-ii-official/ojquestion" xr:uid="{98F61443-6855-47C8-A1C1-CD060F5B59C2}"/>
-    <hyperlink ref="B5" r:id="rId4" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trie/replace-words-official/ojquestion" xr:uid="{B549DC42-23A7-48C2-A22C-317BBE04E61B}"/>
-    <hyperlink ref="B6" r:id="rId5" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trie/maximum-xor-of-two-numbers-in-an-array-official/ojquestion" xr:uid="{243334D3-F178-4530-BFB9-E62EB2B17436}"/>
-    <hyperlink ref="B7" r:id="rId6" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trie/count-pairs-with-xor-in-a-range-official/ojquestion" xr:uid="{301D94A3-BF7E-4A9F-B193-989D0514E9A9}"/>
-    <hyperlink ref="B8" r:id="rId7" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trie/map-sum-pairs-official/ojquestion" xr:uid="{9C381920-ACE6-49E4-ABD8-80221204B063}"/>
-    <hyperlink ref="B9" r:id="rId8" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trie/concatenated-words-official/ojquestion" xr:uid="{98809F49-CA0D-492E-8733-A293C9221800}"/>
-    <hyperlink ref="B10" r:id="rId9" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trie/longest-word-in-dictionary-official/ojquestion" xr:uid="{17194E9F-F529-4FBA-B14E-196499543C77}"/>
-    <hyperlink ref="B11" r:id="rId10" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trie/stream-of-characters-official/ojquestion" xr:uid="{61B1038E-7E54-4F58-BB1B-063087039400}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A2:B45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A36" workbookViewId="0">
       <selection activeCell="B3" sqref="B3:B44"/>
     </sheetView>
   </sheetViews>
@@ -6802,4 +6776,415 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A2:B36"/>
+  <sheetViews>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:A36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="59.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>449</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/next-greater-element-official/ojquestion" xr:uid="{87FD3A23-B754-4247-819F-A63188639CAB}"/>
+    <hyperlink ref="B4" r:id="rId2" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/next-greater-element-left-official/ojquestion" xr:uid="{4180CC0D-6E46-412B-BB97-6F2C7B4D26C0}"/>
+    <hyperlink ref="B5" r:id="rId3" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/next-smaller-element-right-official/ojquestion" xr:uid="{001DDE2A-7B58-4272-88A1-B95092871A34}"/>
+    <hyperlink ref="B6" r:id="rId4" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/next-smaller-element-left-official/ojquestion" xr:uid="{BEAE2BA3-7C9E-4932-B25D-08716B524F10}"/>
+    <hyperlink ref="B7" r:id="rId5" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/next-greater-element-i-official/ojquestion" xr:uid="{5AA31017-3B6C-4190-8239-436BF115A0EA}"/>
+    <hyperlink ref="B8" r:id="rId6" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/next-greater-element-ii-official/ojquestion" xr:uid="{261A595A-9D7C-4369-8418-C2215270A8B8}"/>
+    <hyperlink ref="B9" r:id="rId7" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/largest-area-histogram2-official/ojquestion" xr:uid="{24BBC891-389D-4072-9833-330F9114F269}"/>
+    <hyperlink ref="B10" r:id="rId8" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/maximal-rectangle-official/ojquestion" xr:uid="{64BE7829-27B7-48E4-BA4F-3053A67E1D41}"/>
+    <hyperlink ref="B11" r:id="rId9" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/validate-stack-sequences-official/ojquestion" xr:uid="{688A8C49-2C09-4FAA-B6DC-552A42BF9F9C}"/>
+    <hyperlink ref="B12" r:id="rId10" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/minimum-add-to-make-parentheses-valid-official/ojquestion" xr:uid="{36F6B88B-8DAB-4A01-9D3C-3BADAB479ADB}"/>
+    <hyperlink ref="B13" r:id="rId11" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/remove-outermost-parentheses-official/ojquestion" xr:uid="{4B7845E4-D49A-46D7-BF18-D7409093AD19}"/>
+    <hyperlink ref="B14" r:id="rId12" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/score-of-parentheses-official/ojquestion" xr:uid="{799C5857-1C6B-45FE-8B3A-CAB7C071064B}"/>
+    <hyperlink ref="B15" r:id="rId13" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/reverse-substrings-between-each-pair-of-parentheses-official/ojquestion" xr:uid="{84954448-78C4-4779-839A-43C6CFD7E8F5}"/>
+    <hyperlink ref="B16" r:id="rId14" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/minimum-remove-to-make-valid-parentheses-official/ojquestion" xr:uid="{24507EBF-217F-4FCB-9961-05E8B5A039AF}"/>
+    <hyperlink ref="B17" r:id="rId15" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/online-stock-span-official/ojquestion" xr:uid="{C1711090-7144-46A8-B1D0-E53A3C2EDC1C}"/>
+    <hyperlink ref="B18" r:id="rId16" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/exclusive-time-of-functions-official/ojquestion" xr:uid="{7999D559-34C6-4528-BC05-8898761019C9}"/>
+    <hyperlink ref="B19" r:id="rId17" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/132-pattern-official/ojquestion" xr:uid="{1E571A53-F7D6-4121-9C21-E80CF9AA2778}"/>
+    <hyperlink ref="B20" r:id="rId18" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/asteroid-collision-official/ojquestion" xr:uid="{8F35580B-CD96-4B9B-AF5D-F023C77E9C1F}"/>
+    <hyperlink ref="B21" r:id="rId19" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/remove-k-digits-official/ojquestion" xr:uid="{970FEBE9-0716-4924-9CC2-DFB517E9505E}"/>
+    <hyperlink ref="B22" r:id="rId20" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/remove-duplicate-letters-official/ojquestion" xr:uid="{E42F647E-598B-4580-B5E3-FBA3BDA28062}"/>
+    <hyperlink ref="B23" r:id="rId21" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/trapping-rain-water-official/ojquestion" xr:uid="{27B26838-677E-4D04-9B2C-CB7598170412}"/>
+    <hyperlink ref="B24" r:id="rId22" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/trapping-rain-water-2-official/ojquestion" xr:uid="{9DA3D799-D2F1-4C20-8371-1931B67ECCD8}"/>
+    <hyperlink ref="B25" r:id="rId23" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/number-of-valid-subarrays-official/ojquestion" xr:uid="{464B85CF-3640-48AA-94D4-23D9DA08BBC2}"/>
+    <hyperlink ref="B26" r:id="rId24" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/basic-calculator-official/ojquestion" xr:uid="{1D423A5D-76BF-474D-B4BA-F118B4A791E5}"/>
+    <hyperlink ref="B27" r:id="rId25" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/basic-calculator-ii-official/ojquestion" xr:uid="{2DE15C8F-F385-4DA9-BB08-2405F0094362}"/>
+    <hyperlink ref="B28" r:id="rId26" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/basic-calculator-3-official/ojquestion" xr:uid="{AC707DA2-E4E2-488F-8EC8-181D87D0CE67}"/>
+    <hyperlink ref="B29" r:id="rId27" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/lexicographically-smallest-subsequence-official/ojquestion" xr:uid="{F8DCA947-F3F9-44F9-B656-16E9B0DB5FA3}"/>
+    <hyperlink ref="B30" r:id="rId28" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/design-a-stack-with-increment-operation-official/ojquestion" xr:uid="{056ADEE0-3A3A-4229-B514-75331785371F}"/>
+    <hyperlink ref="B31" r:id="rId29" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/design-circular-deque-official/ojquestion" xr:uid="{371CDA0B-CB92-4C7D-8C6D-262DE7F40094}"/>
+    <hyperlink ref="B32" r:id="rId30" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/max-stack-offical/ojquestion" xr:uid="{FE84D6E4-6D90-4281-A3C6-6B06A04B568E}"/>
+    <hyperlink ref="B33" r:id="rId31" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/check-if-word-is-valid-after-insertion-official/ojquestion" xr:uid="{FBFF2BF1-EE8F-401B-86F2-E146531BD60D}"/>
+    <hyperlink ref="B34" r:id="rId32" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/design-hit-counter-official/ojquestion" xr:uid="{F92DA8A1-3F95-49E9-BFDE-21291D10A370}"/>
+    <hyperlink ref="B35" r:id="rId33" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/number-of-recent-calls-official/ojquestion" xr:uid="{2A60B4A3-5175-478F-9920-6AB7A1E63DA1}"/>
+    <hyperlink ref="B36" r:id="rId34" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/moving-average-from-data-stream-official/ojquestion" xr:uid="{F1F3F1B5-B540-484F-BFE4-5896D6A32CAC}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC154703-7ACF-4C58-B783-B9BD29D8F343}">
+  <dimension ref="B2:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B6" s="1" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B7" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B8" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B9" s="1" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B10" s="1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B11" s="1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trie/implement-trie-official/ojquestion" xr:uid="{4764CADD-C9D7-44A8-9D88-33FF0FA050A7}"/>
+    <hyperlink ref="B3" r:id="rId2" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trie/design-add-and-search-words-data-structure-official/ojquestion" xr:uid="{98FFE7DE-3355-4C30-9D2F-20ECB21881D7}"/>
+    <hyperlink ref="B4" r:id="rId3" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trie/word-search-ii-official/ojquestion" xr:uid="{98F61443-6855-47C8-A1C1-CD060F5B59C2}"/>
+    <hyperlink ref="B5" r:id="rId4" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trie/replace-words-official/ojquestion" xr:uid="{B549DC42-23A7-48C2-A22C-317BBE04E61B}"/>
+    <hyperlink ref="B6" r:id="rId5" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trie/maximum-xor-of-two-numbers-in-an-array-official/ojquestion" xr:uid="{243334D3-F178-4530-BFB9-E62EB2B17436}"/>
+    <hyperlink ref="B7" r:id="rId6" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trie/count-pairs-with-xor-in-a-range-official/ojquestion" xr:uid="{301D94A3-BF7E-4A9F-B193-989D0514E9A9}"/>
+    <hyperlink ref="B8" r:id="rId7" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trie/map-sum-pairs-official/ojquestion" xr:uid="{9C381920-ACE6-49E4-ABD8-80221204B063}"/>
+    <hyperlink ref="B9" r:id="rId8" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trie/concatenated-words-official/ojquestion" xr:uid="{98809F49-CA0D-492E-8733-A293C9221800}"/>
+    <hyperlink ref="B10" r:id="rId9" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trie/longest-word-in-dictionary-official/ojquestion" xr:uid="{17194E9F-F529-4FBA-B14E-196499543C77}"/>
+    <hyperlink ref="B11" r:id="rId10" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trie/stream-of-characters-official/ojquestion" xr:uid="{61B1038E-7E54-4F58-BB1B-063087039400}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>